<commit_message>
Update 80211a i sprzatanie
</commit_message>
<xml_diff>
--- a/Tabelka.xlsx
+++ b/Tabelka.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20010" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="52">
   <si>
     <t>Indeks MCS</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>121.5</t>
+  </si>
+  <si>
+    <t>Szybkosc danychj [Mbps] </t>
+  </si>
+  <si>
+    <t>Tryb</t>
+  </si>
+  <si>
+    <t>BPSK 3/4</t>
   </si>
 </sst>
 </file>
@@ -500,6 +509,54 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -508,54 +565,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -860,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="S1:AB13"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O11" sqref="L1:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,93 +880,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="K1" s="6" t="s">
+      <c r="G1" s="15"/>
+      <c r="K1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="20"/>
-      <c r="S1" s="20" t="s">
+      <c r="Q1" s="10"/>
+      <c r="S1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20" t="s">
+      <c r="V1" s="10"/>
+      <c r="W1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20" t="s">
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20" t="s">
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="20"/>
+      <c r="AB1" s="10"/>
     </row>
     <row r="2" spans="1:28" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
     </row>
     <row r="3" spans="1:28" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
@@ -970,45 +979,45 @@
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="21" t="s">
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="W3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="21" t="s">
+      <c r="X3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="21" t="s">
+      <c r="Y3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="21" t="s">
+      <c r="Z3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="AA3" s="21" t="s">
+      <c r="AA3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="21" t="s">
+      <c r="AB3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1037,10 +1046,10 @@
       <c r="K4" s="4">
         <v>0</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="6">
         <v>0</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N4" s="5">
@@ -1055,10 +1064,10 @@
       <c r="Q4" s="5">
         <v>15</v>
       </c>
-      <c r="S4" s="21">
+      <c r="S4" s="6">
         <v>0</v>
       </c>
-      <c r="T4" s="22" t="s">
+      <c r="T4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="U4" s="5">
@@ -1111,10 +1120,10 @@
       <c r="K5" s="4">
         <v>1</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="6">
         <v>1</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N5" s="5">
@@ -1129,10 +1138,10 @@
       <c r="Q5" s="5">
         <v>30</v>
       </c>
-      <c r="S5" s="21">
+      <c r="S5" s="6">
         <v>1</v>
       </c>
-      <c r="T5" s="22" t="s">
+      <c r="T5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="U5" s="5">
@@ -1185,10 +1194,10 @@
       <c r="K6" s="4">
         <v>2</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="6">
         <v>2</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="M6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="N6" s="5">
@@ -1203,10 +1212,10 @@
       <c r="Q6" s="5">
         <v>45</v>
       </c>
-      <c r="S6" s="21">
+      <c r="S6" s="6">
         <v>2</v>
       </c>
-      <c r="T6" s="22" t="s">
+      <c r="T6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="U6" s="5">
@@ -1259,10 +1268,10 @@
       <c r="K7" s="4">
         <v>3</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="6">
         <v>3</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="M7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="5">
@@ -1277,10 +1286,10 @@
       <c r="Q7" s="5">
         <v>60</v>
       </c>
-      <c r="S7" s="21">
+      <c r="S7" s="6">
         <v>3</v>
       </c>
-      <c r="T7" s="22" t="s">
+      <c r="T7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="U7" s="5">
@@ -1333,10 +1342,10 @@
       <c r="K8" s="4">
         <v>4</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="6">
         <v>4</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="N8" s="5">
@@ -1351,10 +1360,10 @@
       <c r="Q8" s="5">
         <v>90</v>
       </c>
-      <c r="S8" s="21">
+      <c r="S8" s="6">
         <v>4</v>
       </c>
-      <c r="T8" s="22" t="s">
+      <c r="T8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="U8" s="5">
@@ -1407,10 +1416,10 @@
       <c r="K9" s="4">
         <v>5</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="6">
         <v>5</v>
       </c>
-      <c r="M9" s="22" t="s">
+      <c r="M9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="N9" s="5">
@@ -1425,10 +1434,10 @@
       <c r="Q9" s="5">
         <v>120</v>
       </c>
-      <c r="S9" s="21">
+      <c r="S9" s="6">
         <v>5</v>
       </c>
-      <c r="T9" s="22" t="s">
+      <c r="T9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="U9" s="5">
@@ -1481,10 +1490,10 @@
       <c r="K10" s="4">
         <v>6</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="6">
         <v>6</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N10" s="5">
@@ -1499,10 +1508,10 @@
       <c r="Q10" s="5">
         <v>135</v>
       </c>
-      <c r="S10" s="21">
+      <c r="S10" s="6">
         <v>6</v>
       </c>
-      <c r="T10" s="22" t="s">
+      <c r="T10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="U10" s="5">
@@ -1555,10 +1564,10 @@
       <c r="K11" s="4">
         <v>7</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="6">
         <v>7</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="M11" s="7" t="s">
         <v>14</v>
       </c>
       <c r="N11" s="5">
@@ -1573,10 +1582,10 @@
       <c r="Q11" s="5">
         <v>150</v>
       </c>
-      <c r="S11" s="21">
+      <c r="S11" s="6">
         <v>7</v>
       </c>
-      <c r="T11" s="22" t="s">
+      <c r="T11" s="7" t="s">
         <v>14</v>
       </c>
       <c r="U11" s="5">
@@ -1605,10 +1614,10 @@
       </c>
     </row>
     <row r="12" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="S12" s="21">
+      <c r="S12" s="6">
         <v>8</v>
       </c>
-      <c r="T12" s="22" t="s">
+      <c r="T12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="U12" s="5">
@@ -1637,10 +1646,10 @@
       </c>
     </row>
     <row r="13" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="S13" s="21">
+      <c r="S13" s="6">
         <v>9</v>
       </c>
-      <c r="T13" s="22" t="s">
+      <c r="T13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="U13" s="5" t="s">
@@ -1670,289 +1679,289 @@
     </row>
     <row r="17" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J18" s="23">
+      <c r="J18" s="8">
         <v>0</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="8">
         <v>1</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="M18" s="24">
+      <c r="M18" s="9">
         <v>42737</v>
       </c>
-      <c r="N18" s="23" t="s">
+      <c r="N18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O18" s="23" t="s">
+      <c r="O18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="P18" s="23" t="s">
+      <c r="P18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Q18" s="23">
+      <c r="Q18" s="8">
         <v>15</v>
       </c>
-      <c r="R18" s="23" t="s">
+      <c r="R18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="S18" s="23" t="s">
+      <c r="S18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="T18" s="23" t="s">
+      <c r="T18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="U18" s="23">
+      <c r="U18" s="8">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J19" s="23">
+      <c r="J19" s="8">
         <v>1</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K19" s="8">
         <v>1</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M19" s="24">
+      <c r="M19" s="9">
         <v>42737</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N19" s="8">
         <v>13</v>
       </c>
-      <c r="O19" s="23" t="s">
+      <c r="O19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P19" s="23">
+      <c r="P19" s="8">
         <v>27</v>
       </c>
-      <c r="Q19" s="23">
+      <c r="Q19" s="8">
         <v>30</v>
       </c>
-      <c r="R19" s="23" t="s">
+      <c r="R19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="S19" s="23">
+      <c r="S19" s="8">
         <v>65</v>
       </c>
-      <c r="T19" s="23">
+      <c r="T19" s="8">
         <v>117</v>
       </c>
-      <c r="U19" s="23">
+      <c r="U19" s="8">
         <v>130</v>
       </c>
     </row>
     <row r="20" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J20" s="23">
+      <c r="J20" s="8">
         <v>2</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="8">
         <v>1</v>
       </c>
-      <c r="L20" s="23" t="s">
+      <c r="L20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M20" s="24">
+      <c r="M20" s="9">
         <v>42798</v>
       </c>
-      <c r="N20" s="23" t="s">
+      <c r="N20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O20" s="23" t="s">
+      <c r="O20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="P20" s="23" t="s">
+      <c r="P20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Q20" s="23">
+      <c r="Q20" s="8">
         <v>45</v>
       </c>
-      <c r="R20" s="23" t="s">
+      <c r="R20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="S20" s="23" t="s">
+      <c r="S20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="T20" s="23" t="s">
+      <c r="T20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U20" s="23">
+      <c r="U20" s="8">
         <v>195</v>
       </c>
     </row>
     <row r="21" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J21" s="23">
+      <c r="J21" s="8">
         <v>3</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="8">
         <v>1</v>
       </c>
-      <c r="L21" s="23" t="s">
+      <c r="L21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="24">
+      <c r="M21" s="9">
         <v>42737</v>
       </c>
-      <c r="N21" s="23">
+      <c r="N21" s="8">
         <v>26</v>
       </c>
-      <c r="O21" s="23" t="s">
+      <c r="O21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="P21" s="23">
+      <c r="P21" s="8">
         <v>54</v>
       </c>
-      <c r="Q21" s="23">
+      <c r="Q21" s="8">
         <v>60</v>
       </c>
-      <c r="R21" s="23">
+      <c r="R21" s="8">
         <v>117</v>
       </c>
-      <c r="S21" s="23">
+      <c r="S21" s="8">
         <v>130</v>
       </c>
-      <c r="T21" s="23">
+      <c r="T21" s="8">
         <v>234</v>
       </c>
-      <c r="U21" s="23">
+      <c r="U21" s="8">
         <v>260</v>
       </c>
     </row>
     <row r="22" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J22" s="23">
+      <c r="J22" s="8">
         <v>4</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="8">
         <v>1</v>
       </c>
-      <c r="L22" s="23" t="s">
+      <c r="L22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M22" s="24">
+      <c r="M22" s="9">
         <v>42798</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N22" s="8">
         <v>39</v>
       </c>
-      <c r="O22" s="23" t="s">
+      <c r="O22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="8">
         <v>81</v>
       </c>
-      <c r="Q22" s="23">
+      <c r="Q22" s="8">
         <v>90</v>
       </c>
-      <c r="R22" s="23" t="s">
+      <c r="R22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S22" s="23">
+      <c r="S22" s="8">
         <v>195</v>
       </c>
-      <c r="T22" s="23">
+      <c r="T22" s="8">
         <v>351</v>
       </c>
-      <c r="U22" s="23">
+      <c r="U22" s="8">
         <v>390</v>
       </c>
     </row>
     <row r="23" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J23" s="23">
+      <c r="J23" s="8">
         <v>5</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="8">
         <v>1</v>
       </c>
-      <c r="L23" s="23" t="s">
+      <c r="L23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="M23" s="24">
+      <c r="M23" s="9">
         <v>42769</v>
       </c>
-      <c r="N23" s="23">
+      <c r="N23" s="8">
         <v>52</v>
       </c>
-      <c r="O23" s="23" t="s">
+      <c r="O23" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="8">
         <v>108</v>
       </c>
-      <c r="Q23" s="23">
+      <c r="Q23" s="8">
         <v>120</v>
       </c>
-      <c r="R23" s="23">
+      <c r="R23" s="8">
         <v>234</v>
       </c>
-      <c r="S23" s="23">
+      <c r="S23" s="8">
         <v>260</v>
       </c>
-      <c r="T23" s="23">
+      <c r="T23" s="8">
         <v>468</v>
       </c>
-      <c r="U23" s="23">
+      <c r="U23" s="8">
         <v>520</v>
       </c>
     </row>
     <row r="24" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J24" s="23">
+      <c r="J24" s="8">
         <v>6</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="8">
         <v>1</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="M24" s="24">
+      <c r="M24" s="9">
         <v>42798</v>
       </c>
-      <c r="N24" s="23" t="s">
+      <c r="N24" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="O24" s="23">
+      <c r="O24" s="8">
         <v>65</v>
       </c>
-      <c r="P24" s="23" t="s">
+      <c r="P24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="Q24" s="23">
+      <c r="Q24" s="8">
         <v>135</v>
       </c>
-      <c r="R24" s="23" t="s">
+      <c r="R24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S24" s="23" t="s">
+      <c r="S24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="T24" s="23" t="s">
+      <c r="T24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="U24" s="23">
+      <c r="U24" s="8">
         <v>585</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="F1:G2"/>
+    <mergeCell ref="D1:E2"/>
     <mergeCell ref="AA1:AB2"/>
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:V2"/>
     <mergeCell ref="W1:X2"/>
     <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F1:G2"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="L1:L3"/>
-    <mergeCell ref="M1:M3"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="N1:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1961,12 +1970,261 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="I3:K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5">
+        <v>14.4</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>19.5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>21.7</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5">
+        <v>28.9</v>
+      </c>
+      <c r="I7" s="6">
+        <f>I6+1</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5">
+        <v>43.3</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" ref="I8:I13" si="0">I7+1</f>
+        <v>3</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5">
+        <v>52</v>
+      </c>
+      <c r="D9" s="5">
+        <v>57.8</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5">
+        <v>58.5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>65</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>7</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5">
+        <v>65</v>
+      </c>
+      <c r="D11" s="5">
+        <v>72.2</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I12" s="6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I13" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="5">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K3:K5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>